<commit_message>
se modifico el codigo del json handdler ya que no estaba subiendo el archivo json a la base de datos
</commit_message>
<xml_diff>
--- a/app/Plantillas.json/Entrada/Copia de Validez.xlsx
+++ b/app/Plantillas.json/Entrada/Copia de Validez.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uredu.sharepoint.com/sites/DocumentosDatamining/Documentos compartidos/Proyectos/2025/ValidadorDataAnalitic/validadorInteligenteDeDatos/app/Plantillas.json/Entrada/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{BA3CBFE4-CFE3-4522-9363-D5E70D06C822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01A69E90-B0F5-4E1B-8BFE-059B6A5D683C}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{BA3CBFE4-CFE3-4522-9363-D5E70D06C822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB2D90DF-58C8-4B75-8F3E-19ED07E23E5C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{73286C34-7CE1-4AD4-8830-E2B8CFC0150F}"/>
+    <workbookView xWindow="1890" yWindow="1740" windowWidth="20550" windowHeight="11040" xr2:uid="{73286C34-7CE1-4AD4-8830-E2B8CFC0150F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -118,6 +118,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -440,7 +444,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,7 +476,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>45363</v>
+        <v>45373</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -758,15 +762,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92F7F22F-0FD0-4A4D-8E5E-A1D315F9AF91}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F0E02CD-47F6-47CE-BD96-951636156FAB}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5048F621-33F7-483F-A8E8-8E1E8846E424}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B65D98AA-5CD9-47F8-B5D5-4DC8D9A93A5D}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43C721AA-C7F9-40AC-A949-FAA133593974}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE93BFC0-2742-40E5-8B7C-1540CCE9DBA7}"/>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>